<commit_message>
Commiting Banker's cheque and Customer Creation
</commit_message>
<xml_diff>
--- a/Data/UnAuth_Customers.xlsx
+++ b/Data/UnAuth_Customers.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xcelliti4\IdeaProjects\Retail Ops\Data\"/>
     </mc:Choice>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
   <si>
     <t>TC</t>
   </si>
@@ -32,11 +32,24 @@
   <si>
     <t>authorized already</t>
   </si>
+  <si>
+    <t>118448</t>
+  </si>
+  <si>
+    <t>17704491</t>
+  </si>
+  <si>
+    <t>1005</t>
+  </si>
+  <si>
+    <t>17704492</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -349,7 +362,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C99"/>
+  <dimension ref="A1:C101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
@@ -357,7 +370,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -1445,6 +1458,28 @@
         <v>1050</v>
       </c>
     </row>
+    <row r="100">
+      <c r="A100" t="s">
+        <v>4</v>
+      </c>
+      <c r="B100" t="s">
+        <v>5</v>
+      </c>
+      <c r="C100" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="s">
+        <v>4</v>
+      </c>
+      <c r="B101" t="s">
+        <v>7</v>
+      </c>
+      <c r="C101" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Commiting Customer Creation and Account Creation
</commit_message>
<xml_diff>
--- a/Data/UnAuth_Customers.xlsx
+++ b/Data/UnAuth_Customers.xlsx
@@ -3,23 +3,24 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xcelliti4\IdeaProjects\Retail Ops\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Selenium Workspace Functional Testing\Retail Ops\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet0" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet0" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="26">
   <si>
     <t>TC</t>
   </si>
@@ -43,13 +44,66 @@
   </si>
   <si>
     <t>17704492</t>
+  </si>
+  <si>
+    <t>17704511</t>
+  </si>
+  <si>
+    <t>17704524</t>
+  </si>
+  <si>
+    <t>118450</t>
+  </si>
+  <si>
+    <t>17704525</t>
+  </si>
+  <si>
+    <t>118451</t>
+  </si>
+  <si>
+    <t>17704526</t>
+  </si>
+  <si>
+    <t>17704530</t>
+  </si>
+  <si>
+    <t>17704531</t>
+  </si>
+  <si>
+    <t>17704532</t>
+  </si>
+  <si>
+    <t>17704540</t>
+  </si>
+  <si>
+    <t>17704541</t>
+  </si>
+  <si>
+    <t>17704543</t>
+  </si>
+  <si>
+    <t>17704590</t>
+  </si>
+  <si>
+    <t>17704591</t>
+  </si>
+  <si>
+    <t>17704592</t>
+  </si>
+  <si>
+    <t>118452</t>
+  </si>
+  <si>
+    <t>17704593</t>
+  </si>
+  <si>
+    <t>17704594</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -362,15 +416,96 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C101"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C111"/>
+  <sheetViews>
+    <sheetView topLeftCell="A91" workbookViewId="0">
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
+    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -1458,7 +1593,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="100">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>4</v>
       </c>
@@ -1469,7 +1604,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="101">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>4</v>
       </c>
@@ -1477,6 +1612,116 @@
         <v>7</v>
       </c>
       <c r="C101" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>4</v>
+      </c>
+      <c r="B102" t="s">
+        <v>8</v>
+      </c>
+      <c r="C102" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>4</v>
+      </c>
+      <c r="B103" t="s">
+        <v>9</v>
+      </c>
+      <c r="C103" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>10</v>
+      </c>
+      <c r="B104" t="s">
+        <v>11</v>
+      </c>
+      <c r="C104" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>12</v>
+      </c>
+      <c r="B105" t="s">
+        <v>13</v>
+      </c>
+      <c r="C105" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>4</v>
+      </c>
+      <c r="B106" t="s">
+        <v>14</v>
+      </c>
+      <c r="C106" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>10</v>
+      </c>
+      <c r="B107" t="s">
+        <v>15</v>
+      </c>
+      <c r="C107" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>12</v>
+      </c>
+      <c r="B108" t="s">
+        <v>16</v>
+      </c>
+      <c r="C108" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>4</v>
+      </c>
+      <c r="B109" t="s">
+        <v>17</v>
+      </c>
+      <c r="C109" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>10</v>
+      </c>
+      <c r="B110" t="s">
+        <v>18</v>
+      </c>
+      <c r="C110" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>12</v>
+      </c>
+      <c r="B111" t="s">
+        <v>19</v>
+      </c>
+      <c r="C111" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Commiting scripts + their data
</commit_message>
<xml_diff>
--- a/Data/UnAuth_Customers.xlsx
+++ b/Data/UnAuth_Customers.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Selenium Workspace Functional Testing\Retail Ops\Data\"/>
     </mc:Choice>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="20">
   <si>
     <t>TC</t>
   </si>
@@ -82,49 +82,12 @@
   </si>
   <si>
     <t>17704543</t>
-  </si>
-  <si>
-    <t>118463</t>
-  </si>
-  <si>
-    <t>17707515</t>
-  </si>
-  <si>
-    <t>1010</t>
-  </si>
-  <si>
-    <t>17707516</t>
-  </si>
-  <si>
-    <t>1003</t>
-  </si>
-  <si>
-    <t>17707517</t>
-  </si>
-  <si>
-    <t>1007</t>
-  </si>
-  <si>
-    <t>118464</t>
-  </si>
-  <si>
-    <t>17707519</t>
-  </si>
-  <si>
-    <t>118465</t>
-  </si>
-  <si>
-    <t>17707520</t>
-  </si>
-  <si>
-    <t>1011</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -437,7 +400,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:C11"/>
@@ -454,61 +417,6 @@
       </c>
       <c r="C1" t="s">
         <v>2</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s">
-        <v>29</v>
-      </c>
-      <c r="B6" t="s">
-        <v>30</v>
-      </c>
-      <c r="C6" t="s">
-        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -539,7 +447,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
+    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>